<commit_message>
#3 support synchro.npy in excel configuration
update documentation with ppt links
</commit_message>
<xml_diff>
--- a/Templates/config.xlsx
+++ b/Templates/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Flight-Plan" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
     <t>drone</t>
   </si>
@@ -100,9 +100,6 @@
     <t>IRDrone</t>
   </si>
   <si>
-    <t>N 45.16969 E 3.39996</t>
-  </si>
-  <si>
     <t>FLY202201251159</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>s  (A value of -1 if no timelapse.)</t>
   </si>
   <si>
-    <t xml:space="preserve">  V1.0   keep this value at zero.</t>
-  </si>
-  <si>
     <t>Imatriculation</t>
   </si>
   <si>
@@ -200,6 +194,18 @@
   </si>
   <si>
     <t>Value given by synchro</t>
+  </si>
+  <si>
+    <t>Synchro/synchro.npy</t>
+  </si>
+  <si>
+    <t>synchro file (.npy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> keep this value at zero.</t>
+  </si>
+  <si>
+    <t>Pleas provide path after executing synchro.bat</t>
   </si>
 </sst>
 </file>
@@ -209,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,27 +261,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
@@ -300,6 +285,64 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -343,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -543,11 +586,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -609,8 +667,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -623,48 +679,62 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,16 +1045,16 @@
   <dimension ref="A1:L728"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" customWidth="1"/>
-    <col min="2" max="2" width="65.90625" customWidth="1"/>
-    <col min="6" max="6" width="4.08984375" customWidth="1"/>
-    <col min="9" max="9" width="47.453125" customWidth="1"/>
-    <col min="10" max="10" width="53.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="65.88671875" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" customWidth="1"/>
+    <col min="9" max="9" width="47.44140625" customWidth="1"/>
+    <col min="10" max="10" width="53.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="149.4" customHeight="1" thickBot="1">
@@ -1003,7 +1073,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -1019,7 +1089,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
@@ -1037,7 +1107,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>26</v>
@@ -1054,71 +1124,66 @@
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25">
         <v>3</v>
       </c>
-      <c r="G5" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="38"/>
+      <c r="G5" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="56"/>
+      <c r="I5" s="57"/>
       <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="4">
-        <v>520</v>
-      </c>
-      <c r="C6" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="25">
         <v>4</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="43">
-        <v>44586.499872685185</v>
-      </c>
-      <c r="C7" s="37" t="s">
+      <c r="A7" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="37">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25">
         <v>5</v>
       </c>
-      <c r="G7" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="G7" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2">
         <v>0.4513888888888889</v>
@@ -1138,10 +1203,10 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
@@ -1156,10 +1221,10 @@
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1">
       <c r="A10" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -1188,7 +1253,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>20</v>
@@ -1206,9 +1271,9 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="24"/>
@@ -1224,29 +1289,29 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="40">
+        <v>39</v>
+      </c>
+      <c r="B14" s="37">
         <v>2</v>
       </c>
-      <c r="C14" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37">
+      <c r="C14" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49">
         <v>3</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="52">
+      <c r="A15" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="44">
         <v>0</v>
       </c>
       <c r="C15" s="24" t="s">
@@ -1257,8 +1322,8 @@
       <c r="F15" s="25">
         <v>4</v>
       </c>
-      <c r="G15" s="32" t="s">
-        <v>45</v>
+      <c r="G15" s="51" t="s">
+        <v>62</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
@@ -1266,7 +1331,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="24"/>
@@ -1282,7 +1347,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="7">
         <v>150</v>
@@ -1332,7 +1397,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>21</v>
@@ -1350,9 +1415,9 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="24"/>
@@ -1368,9 +1433,9 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="48">
+        <v>39</v>
+      </c>
+      <c r="B22" s="42">
         <v>3</v>
       </c>
       <c r="C22" s="24" t="s">
@@ -1386,13 +1451,11 @@
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="42">
-        <v>3894.74037</v>
-      </c>
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="45"/>
       <c r="C23" s="31" t="s">
         <v>24</v>
       </c>
@@ -1401,10 +1464,10 @@
       <c r="F23" s="25">
         <v>4</v>
       </c>
-      <c r="G23" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="H23" s="24"/>
+      <c r="G23" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" s="52"/>
       <c r="I23" s="24"/>
       <c r="J23" s="24"/>
     </row>
@@ -1412,7 +1475,7 @@
       <c r="A24" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -1440,15 +1503,15 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
-      <c r="F26" s="37">
+      <c r="F26" s="35">
         <v>1</v>
       </c>
       <c r="G26" s="24"/>
@@ -1458,15 +1521,15 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="54" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="37">
+      <c r="F27" s="35">
         <v>2</v>
       </c>
       <c r="G27" s="24"/>
@@ -1478,13 +1541,13 @@
       <c r="A28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="54" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="37">
+      <c r="F28" s="35">
         <v>3</v>
       </c>
       <c r="G28" s="24"/>
@@ -1494,9 +1557,9 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="34"/>
+        <v>53</v>
+      </c>
+      <c r="B29" s="32"/>
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
@@ -1512,7 +1575,7 @@
       <c r="A30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="34"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
@@ -1528,7 +1591,7 @@
       <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="34"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -1542,15 +1605,15 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="53" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
-      <c r="F32" s="37">
+      <c r="F32" s="35">
         <v>7</v>
       </c>
       <c r="G32" s="24"/>
@@ -1562,13 +1625,13 @@
       <c r="A33" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="54" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="37">
+      <c r="F33" s="35">
         <v>8</v>
       </c>
       <c r="G33" s="24"/>
@@ -1577,10 +1640,10 @@
       <c r="J33" s="24"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="45">
+      <c r="A34" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="39">
         <v>720</v>
       </c>
       <c r="C34" s="24" t="s">
@@ -1597,10 +1660,10 @@
       <c r="J34" s="24"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -1613,10 +1676,10 @@
       <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -1644,10 +1707,10 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
@@ -1662,7 +1725,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B39" s="4">
         <v>10</v>
@@ -1682,7 +1745,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="4">
         <v>10</v>
@@ -1702,7 +1765,7 @@
     </row>
     <row r="41" spans="1:10" s="26" customFormat="1" ht="15" thickBot="1">
       <c r="A41" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B41" s="9">
         <v>65</v>
@@ -1720,12 +1783,20 @@
       <c r="I41" s="23"/>
       <c r="J41" s="23"/>
     </row>
-    <row r="42" spans="1:10" s="26" customFormat="1">
+    <row r="42" spans="1:10" s="26" customFormat="1" ht="15" thickBot="1">
+      <c r="A42" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="61" t="s">
+        <v>60</v>
+      </c>
       <c r="C42" s="23"/>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
       <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
+      <c r="G42" s="52" t="s">
+        <v>63</v>
+      </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
       <c r="J42" s="23"/>
@@ -5153,7 +5224,7 @@
     <row r="727" s="26" customFormat="1"/>
     <row r="728" s="26" customFormat="1"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState ref="A9:C20">
     <sortCondition sortBy="icon" ref="A13"/>
   </sortState>

</xml_diff>